<commit_message>
use data for AHP
</commit_message>
<xml_diff>
--- a/result/Region_Estimaiton_Result.xlsx
+++ b/result/Region_Estimaiton_Result.xlsx
@@ -359,7 +359,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -368,87 +368,84 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Region</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>China</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Y_Import</t>
+          <t>EU</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>r_c</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>r_p</t>
+          <t>India</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>High-Income</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8.422108782381621</v>
+        <v>-9.932487581726193</v>
       </c>
       <c r="C2" t="n">
-        <v>-6.123724356957945</v>
+        <v>24.98504778026656</v>
       </c>
       <c r="D2" t="n">
-        <v>9.382223764206376</v>
-      </c>
-      <c r="E2" t="n">
-        <v>10.01173683715106</v>
+        <v>-15.05256019854037</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Middle-Income</t>
+          <t>Y_Import</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8.692763041394276</v>
+        <v>6.97521704121815</v>
       </c>
       <c r="C3" t="n">
-        <v>6.123724356957945</v>
+        <v>-14.14170446634398</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.400254790115887</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-0.4526787302125923</v>
+        <v>7.166487425125831</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Low-Income</t>
+          <t>r_c</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-17.1148718237759</v>
+        <v>-5.032224880158286</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>10.84554644021556</v>
       </c>
       <c r="D4" t="n">
-        <v>-8.981968974090488</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-9.559058106938471</v>
+        <v>-5.813321560057277</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>r_p</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-3.436828665498592</v>
+      </c>
+      <c r="C5" t="n">
+        <v>8.7831677131497</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-5.346339047651106</v>
       </c>
     </row>
   </sheetData>
@@ -462,7 +459,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,87 +468,84 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Region</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>China</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Y_Import</t>
+          <t>EU</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>r_c</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>r_p</t>
+          <t>India</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>High-Income</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6958956033794405</v>
+        <v>-1.14860886739979</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.224744871391589</v>
+        <v>1.238235081695834</v>
       </c>
       <c r="D2" t="n">
-        <v>1.250547895131892</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1.252069206397946</v>
+        <v>-1.302697326032186</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Middle-Income</t>
+          <t>Y_Import</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7182590177866296</v>
+        <v>1.5959637597411</v>
       </c>
       <c r="C3" t="n">
-        <v>1.224744871391589</v>
+        <v>-1.551424851074756</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.05334958938044677</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-0.05661206519005899</v>
+        <v>1.509890094087287</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Low-Income</t>
+          <t>r_c</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.41415462116607</v>
+        <v>-0.3531651820238457</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.2301166437257283</v>
       </c>
       <c r="D4" t="n">
-        <v>-1.197198305751445</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-1.195457141207887</v>
+        <v>-0.13315276200683</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>r_p</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-0.09418971031746368</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.08307312565319393</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.07404000604827089</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data of AHP
</commit_message>
<xml_diff>
--- a/result/Region_Estimaiton_Result.xlsx
+++ b/result/Region_Estimaiton_Result.xlsx
@@ -359,7 +359,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -368,83 +368,86 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Region</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>EU</t>
+          <t>Y_Import</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>r_c</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>r_p</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>-9.932487581726193</v>
       </c>
       <c r="C2" t="n">
-        <v>24.98504778026656</v>
+        <v>6.97521704121815</v>
       </c>
       <c r="D2" t="n">
-        <v>-15.05256019854037</v>
+        <v>-5.032224880158286</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-3.436828665498592</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Y_Import</t>
+          <t>EU</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.97521704121815</v>
+        <v>24.98504778026656</v>
       </c>
       <c r="C3" t="n">
         <v>-14.14170446634398</v>
       </c>
       <c r="D3" t="n">
-        <v>7.166487425125831</v>
+        <v>10.84554644021556</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8.7831677131497</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>r_c</t>
+          <t>India</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-5.032224880158286</v>
+        <v>-15.05256019854037</v>
       </c>
       <c r="C4" t="n">
-        <v>10.84554644021556</v>
+        <v>7.166487425125831</v>
       </c>
       <c r="D4" t="n">
         <v>-5.813321560057277</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>r_p</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>-3.436828665498592</v>
-      </c>
-      <c r="C5" t="n">
-        <v>8.7831677131497</v>
-      </c>
-      <c r="D5" t="n">
+      <c r="E4" t="n">
         <v>-5.346339047651106</v>
       </c>
     </row>
@@ -459,7 +462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,84 +471,87 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Region</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>EU</t>
+          <t>Y_Import</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>r_c</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>r_p</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.14860886739979</v>
+        <v>-0.5583085299284382</v>
       </c>
       <c r="C2" t="n">
-        <v>1.238235081695834</v>
+        <v>0.697521704121815</v>
       </c>
       <c r="D2" t="n">
-        <v>-1.302697326032186</v>
+        <v>-0.6556144016474311</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-0.549069353459124</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Y_Import</t>
+          <t>EU</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.5959637597411</v>
+        <v>1.404418095830945</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.551424851074756</v>
+        <v>-1.414170446634398</v>
       </c>
       <c r="D3" t="n">
-        <v>1.509890094087287</v>
+        <v>1.412992584647309</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.403202977790146</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>r_c</t>
+          <t>India</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.3531651820238457</v>
+        <v>-0.846109565902507</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2301166437257283</v>
+        <v>0.7166487425125831</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.13315276200683</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>r_p</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>-0.09418971031746368</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.08307312565319393</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.07404000604827089</v>
+        <v>-0.7573781829998781</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.8541336243310218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>